<commit_message>
complete insert method for spreadsheet
</commit_message>
<xml_diff>
--- a/singles_tournament_2021.xlsx
+++ b/singles_tournament_2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adarsh\Documents\python\Personal_Projects\Auto_Tennis_Log[0]\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DF4146D-82C5-43E5-B277-086ADA3728B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7966C52-8F68-4BA3-966A-8E78FF7A28C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14190" yWindow="30" windowWidth="14610" windowHeight="15135" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -371,7 +371,7 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>